<commit_message>
Added 2019 NFL Conference Championship forecasts
</commit_message>
<xml_diff>
--- a/NFL2019/Weekly Forecasts/WeekDivMatrix.xlsx
+++ b/NFL2019/Weekly Forecasts/WeekDivMatrix.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\MerrerPredictifier\MerrerPredictifier\NFL2019\Weekly Forecasts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2A80DB8-D7D1-4694-8FD1-74B2538DEEB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EE9B857-B4AE-4E27-AAFB-29ED1C7D23B3}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10460" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -704,31 +704,7 @@
     <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="10" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -816,6 +792,30 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="166" fontId="16" fillId="10" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1198,16 +1198,16 @@
       <c r="E3" s="18"/>
       <c r="F3" s="18"/>
       <c r="G3" s="18"/>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="49" t="s">
         <v>42</v>
       </c>
-      <c r="I3" s="20"/>
+      <c r="I3" s="50"/>
       <c r="J3" s="18"/>
       <c r="K3" s="18"/>
       <c r="L3" s="18"/>
       <c r="M3" s="18"/>
       <c r="N3" s="18"/>
-      <c r="O3" s="21"/>
+      <c r="O3" s="19"/>
     </row>
     <row r="4" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B4" s="17"/>
@@ -1216,16 +1216,16 @@
       <c r="E4" s="18"/>
       <c r="F4" s="18"/>
       <c r="G4" s="18"/>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="51" t="s">
         <v>43</v>
       </c>
-      <c r="I4" s="23"/>
+      <c r="I4" s="52"/>
       <c r="J4" s="18"/>
       <c r="K4" s="18"/>
       <c r="L4" s="18"/>
       <c r="M4" s="18"/>
       <c r="N4" s="18"/>
-      <c r="O4" s="21"/>
+      <c r="O4" s="19"/>
     </row>
     <row r="5" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B5" s="17"/>
@@ -1234,16 +1234,16 @@
       <c r="E5" s="18"/>
       <c r="F5" s="18"/>
       <c r="G5" s="18"/>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="53" t="s">
         <v>44</v>
       </c>
-      <c r="I5" s="25"/>
+      <c r="I5" s="54"/>
       <c r="J5" s="18"/>
       <c r="K5" s="18"/>
       <c r="L5" s="18"/>
       <c r="M5" s="18"/>
       <c r="N5" s="18"/>
-      <c r="O5" s="21"/>
+      <c r="O5" s="19"/>
     </row>
     <row r="6" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B6" s="17"/>
@@ -1252,16 +1252,16 @@
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="18"/>
-      <c r="H6" s="26" t="s">
+      <c r="H6" s="55" t="s">
         <v>21</v>
       </c>
-      <c r="I6" s="27"/>
+      <c r="I6" s="56"/>
       <c r="J6" s="18"/>
       <c r="K6" s="18"/>
       <c r="L6" s="18"/>
       <c r="M6" s="18"/>
       <c r="N6" s="18"/>
-      <c r="O6" s="21"/>
+      <c r="O6" s="19"/>
     </row>
     <row r="7" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B7" s="17"/>
@@ -1271,13 +1271,13 @@
       <c r="F7" s="18"/>
       <c r="G7" s="18"/>
       <c r="H7" s="18"/>
-      <c r="I7" s="28"/>
+      <c r="I7" s="20"/>
       <c r="J7" s="18"/>
       <c r="K7" s="18"/>
       <c r="L7" s="18"/>
       <c r="M7" s="18"/>
       <c r="N7" s="18"/>
-      <c r="O7" s="21"/>
+      <c r="O7" s="19"/>
     </row>
     <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="17"/>
@@ -1286,10 +1286,10 @@
       <c r="E8" s="18"/>
       <c r="F8" s="18"/>
       <c r="G8" s="18"/>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="I8" s="30" t="s">
+      <c r="I8" s="22" t="s">
         <v>26</v>
       </c>
       <c r="J8" s="18"/>
@@ -1297,7 +1297,7 @@
       <c r="L8" s="18"/>
       <c r="M8" s="18"/>
       <c r="N8" s="18"/>
-      <c r="O8" s="21"/>
+      <c r="O8" s="19"/>
     </row>
     <row r="9" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B9" s="17"/>
@@ -1305,19 +1305,19 @@
       <c r="D9" s="18"/>
       <c r="E9" s="18"/>
       <c r="F9" s="18"/>
-      <c r="G9" s="31"/>
-      <c r="H9" s="32">
+      <c r="G9" s="23"/>
+      <c r="H9" s="24">
         <v>29.712966999999999</v>
       </c>
-      <c r="I9" s="33">
+      <c r="I9" s="25">
         <v>24.4853624</v>
       </c>
-      <c r="J9" s="34"/>
-      <c r="K9" s="35"/>
+      <c r="J9" s="26"/>
+      <c r="K9" s="27"/>
       <c r="L9" s="18"/>
       <c r="M9" s="18"/>
       <c r="N9" s="18"/>
-      <c r="O9" s="21"/>
+      <c r="O9" s="19"/>
     </row>
     <row r="10" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B10" s="17"/>
@@ -1325,239 +1325,239 @@
       <c r="D10" s="18"/>
       <c r="E10" s="18"/>
       <c r="F10" s="18"/>
-      <c r="G10" s="35"/>
+      <c r="G10" s="27"/>
       <c r="H10" s="18"/>
       <c r="I10" s="18"/>
       <c r="J10" s="18"/>
-      <c r="K10" s="35"/>
+      <c r="K10" s="27"/>
       <c r="L10" s="18"/>
       <c r="M10" s="18"/>
       <c r="N10" s="18"/>
-      <c r="O10" s="21"/>
+      <c r="O10" s="19"/>
     </row>
     <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" s="17"/>
       <c r="C11" s="18"/>
       <c r="D11" s="18"/>
       <c r="E11" s="18"/>
-      <c r="F11" s="29" t="s">
+      <c r="F11" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G11" s="39" t="s">
+      <c r="G11" s="31" t="s">
         <v>22</v>
       </c>
       <c r="H11" s="18"/>
       <c r="I11" s="18"/>
-      <c r="J11" s="36" t="s">
+      <c r="J11" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="K11" s="42" t="s">
+      <c r="K11" s="34" t="s">
         <v>27</v>
       </c>
       <c r="L11" s="18"/>
       <c r="M11" s="18"/>
       <c r="N11" s="18"/>
-      <c r="O11" s="21"/>
+      <c r="O11" s="19"/>
     </row>
     <row r="12" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B12" s="17"/>
       <c r="C12" s="18"/>
-      <c r="D12" s="31"/>
-      <c r="E12" s="34"/>
-      <c r="F12" s="37">
+      <c r="D12" s="23"/>
+      <c r="E12" s="26"/>
+      <c r="F12" s="29">
         <v>29.651449</v>
       </c>
-      <c r="G12" s="38">
+      <c r="G12" s="30">
         <v>23.9714314</v>
       </c>
       <c r="H12" s="18"/>
       <c r="I12" s="18"/>
-      <c r="J12" s="37">
+      <c r="J12" s="29">
         <v>26.6049756</v>
       </c>
-      <c r="K12" s="38">
+      <c r="K12" s="30">
         <v>19.7583944</v>
       </c>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="35"/>
-      <c r="O12" s="21"/>
+      <c r="L12" s="26"/>
+      <c r="M12" s="26"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="19"/>
     </row>
     <row r="13" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B13" s="17"/>
       <c r="C13" s="18"/>
-      <c r="D13" s="35"/>
+      <c r="D13" s="27"/>
       <c r="E13" s="18"/>
       <c r="F13" s="18"/>
-      <c r="G13" s="35"/>
+      <c r="G13" s="27"/>
       <c r="H13" s="18"/>
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
-      <c r="K13" s="35"/>
+      <c r="K13" s="27"/>
       <c r="L13" s="18"/>
       <c r="M13" s="18"/>
-      <c r="N13" s="35"/>
-      <c r="O13" s="21"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="19"/>
     </row>
     <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" s="17"/>
-      <c r="C14" s="39" t="s">
+      <c r="C14" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="45" t="s">
+      <c r="D14" s="37" t="s">
         <v>24</v>
       </c>
       <c r="E14" s="18"/>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="21" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="44" t="s">
+      <c r="G14" s="36" t="s">
         <v>25</v>
       </c>
       <c r="H14" s="18"/>
       <c r="I14" s="18"/>
-      <c r="J14" s="36" t="s">
+      <c r="J14" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="48" t="s">
+      <c r="K14" s="40" t="s">
         <v>29</v>
       </c>
       <c r="L14" s="18"/>
-      <c r="M14" s="42" t="s">
-        <v>27</v>
-      </c>
-      <c r="N14" s="41" t="s">
+      <c r="M14" s="34" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O14" s="21"/>
+      <c r="O14" s="19"/>
     </row>
     <row r="15" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B15" s="17"/>
-      <c r="C15" s="37">
+      <c r="C15" s="29">
         <v>29.489412600000001</v>
       </c>
-      <c r="D15" s="49">
+      <c r="D15" s="41">
         <v>20.8242844</v>
       </c>
       <c r="E15" s="18"/>
-      <c r="F15" s="37">
+      <c r="F15" s="29">
         <v>30.588047</v>
       </c>
-      <c r="G15" s="38">
+      <c r="G15" s="30">
         <v>20.202910200000002</v>
       </c>
       <c r="H15" s="18"/>
       <c r="I15" s="18"/>
-      <c r="J15" s="37">
+      <c r="J15" s="29">
         <v>25.876151</v>
       </c>
-      <c r="K15" s="38">
+      <c r="K15" s="30">
         <v>21.930274000000001</v>
       </c>
       <c r="L15" s="18"/>
-      <c r="M15" s="37">
+      <c r="M15" s="29">
         <v>23.5925324</v>
       </c>
-      <c r="N15" s="49">
+      <c r="N15" s="41">
         <v>21.722424400000001</v>
       </c>
-      <c r="O15" s="21"/>
+      <c r="O15" s="19"/>
     </row>
     <row r="16" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B16" s="17"/>
       <c r="C16" s="18"/>
-      <c r="D16" s="35"/>
+      <c r="D16" s="27"/>
       <c r="E16" s="18"/>
       <c r="F16" s="18"/>
-      <c r="G16" s="35"/>
+      <c r="G16" s="27"/>
       <c r="H16" s="18"/>
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
-      <c r="K16" s="35"/>
+      <c r="K16" s="27"/>
       <c r="L16" s="18"/>
       <c r="M16" s="18"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="21"/>
+      <c r="N16" s="27"/>
+      <c r="O16" s="19"/>
     </row>
     <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" s="17"/>
-      <c r="C17" s="45" t="s">
-        <v>24</v>
-      </c>
-      <c r="D17" s="40" t="s">
+      <c r="C17" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="D17" s="32" t="s">
         <v>47</v>
       </c>
       <c r="E17" s="18"/>
-      <c r="F17" s="43" t="s">
+      <c r="F17" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="G17" s="44" t="s">
+      <c r="G17" s="36" t="s">
         <v>25</v>
       </c>
       <c r="H17" s="18"/>
       <c r="I17" s="18"/>
-      <c r="J17" s="47" t="s">
+      <c r="J17" s="39" t="s">
         <v>46</v>
       </c>
-      <c r="K17" s="48" t="s">
+      <c r="K17" s="40" t="s">
         <v>29</v>
       </c>
       <c r="L17" s="18"/>
-      <c r="M17" s="46" t="s">
+      <c r="M17" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="N17" s="41" t="s">
+      <c r="N17" s="33" t="s">
         <v>28</v>
       </c>
-      <c r="O17" s="21"/>
+      <c r="O17" s="19"/>
     </row>
     <row r="18" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B18" s="17"/>
-      <c r="C18" s="55">
+      <c r="C18" s="47">
         <v>22</v>
       </c>
-      <c r="D18" s="56">
+      <c r="D18" s="48">
         <v>19</v>
       </c>
       <c r="E18" s="18"/>
-      <c r="F18" s="53">
+      <c r="F18" s="45">
         <v>13</v>
       </c>
-      <c r="G18" s="54">
+      <c r="G18" s="46">
         <v>20</v>
       </c>
       <c r="H18" s="18"/>
       <c r="I18" s="18"/>
-      <c r="J18" s="53">
-        <v>20</v>
-      </c>
-      <c r="K18" s="54">
+      <c r="J18" s="45">
+        <v>20</v>
+      </c>
+      <c r="K18" s="46">
         <v>26</v>
       </c>
       <c r="L18" s="18"/>
-      <c r="M18" s="53">
+      <c r="M18" s="45">
         <v>9</v>
       </c>
-      <c r="N18" s="54">
-        <v>17</v>
-      </c>
-      <c r="O18" s="21"/>
+      <c r="N18" s="46">
+        <v>17</v>
+      </c>
+      <c r="O18" s="19"/>
     </row>
     <row r="19" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="B19" s="50"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-      <c r="G19" s="51"/>
-      <c r="H19" s="51"/>
-      <c r="I19" s="51"/>
-      <c r="J19" s="51"/>
-      <c r="K19" s="51"/>
-      <c r="L19" s="51"/>
-      <c r="M19" s="51"/>
-      <c r="N19" s="51"/>
-      <c r="O19" s="52"/>
+      <c r="B19" s="42"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
+      <c r="K19" s="43"/>
+      <c r="L19" s="43"/>
+      <c r="M19" s="43"/>
+      <c r="N19" s="43"/>
+      <c r="O19" s="44"/>
     </row>
   </sheetData>
   <mergeCells count="4">

</xml_diff>